<commit_message>
Added comments to the ShawnTestingWebsites.py
</commit_message>
<xml_diff>
--- a/ShawnTestData.xlsx
+++ b/ShawnTestData.xlsx
@@ -379,6 +379,11 @@
           <t>Tech</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -437,52 +442,39 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Microsoft Jobs, Employment in Denver, CO | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed.com
+</t>
+        </is>
+      </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/company/microsoft/jobs</t>
+          <t>https://www.indeed.com/q-Microsoft-l-Denver,-CO-jobs.html</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>508,000+ Microsoft jobs in United States (16,994 new)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="n">
-        <v>689</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/microsoft-jobs</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
           <t>Microsoft Jobs and Careers | Indeed.com</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t xml:space="preserve">white@2x.png
 white@2x.png
@@ -491,18 +483,36 @@
 </t>
         </is>
       </c>
+      <c r="C5" t="n">
+        <v>282</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>28</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/cmp/Microsoft/jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>294</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/cmp/Microsoft/jobs</t>
+          <t>https://www.linkedin.com/company/microsoft/jobs</t>
         </is>
       </c>
     </row>
@@ -541,9 +551,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">donkey@jackasswhisperer.com
-u003edonkey@jackasswhisperer.com
-mingraham@theladders.com.
+          <t xml:space="preserve">mingraham@theladders.com.
 mingraham@theladders.com
 mlepore@theladders.com.
 mlepore@theladders.com
@@ -566,13 +574,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2115</v>
+        <v>2144</v>
       </c>
       <c r="D8" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" t="n">
-        <v>281</v>
+        <v>318</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Adding Google search Module
</commit_message>
<xml_diff>
--- a/ShawnTestData.xlsx
+++ b/ShawnTestData.xlsx
@@ -388,203 +388,186 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Careers at Microsoft | Microsoft jobs</t>
+          <t>Tree - Wikipedia</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">askgta@microsoft.com
+          <t xml:space="preserve">tokens@tffin
 </t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>550</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://careers.microsoft.com/us/en/</t>
+          <t>https://en.wikipedia.org/wiki/Tree</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Apache Tomcat - Error report</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">react@16.3.2
-dom@16.3.2
-types@15.6.2
-</t>
-        </is>
-      </c>
+          <t>ss-standard-user</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.glassdoor.com/Jobs/Microsoft-Jobs-E1651.htm</t>
+          <t>https://www.arborday.org/trees/treeGuide/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Microsoft Jobs, Employment in Denver, CO | Indeed.com</t>
+          <t>tree | Structure, Uses, Importance, &amp; Facts | Britannica</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed.com
+          <t xml:space="preserve">1791028@640x480
 </t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1100</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/q-Microsoft-l-Denver,-CO-jobs.html</t>
+          <t>https://www.britannica.com/plant/tree</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Microsoft Jobs and Careers | Indeed.com</t>
+          <t>Anniversary-logo-white</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">white@2x.png
-white@2x.png
-658ba2886a9642c2b8c035add5a02b63@sentry.indeed.com
-u002f9282b91fa44845a98549f9a94b9326b2@sentry.indeed.com
+          <t xml:space="preserve">info@trees.org
+info@trees.org
 </t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>282</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/cmp/Microsoft/jobs</t>
+          <t>https://trees.org/</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@onetreeplanted.org
+hello@onetreeplanted.org
+hello@onetreeplanted.org
+hello@onetreeplanted.org
+</t>
+        </is>
+      </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/company/microsoft/jobs</t>
+          <t>https://onetreeplanted.org/pages/why-trees</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Not Found | SimplyHired</t>
+          <t>Top 22 Benefits of Trees | TreePeople</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">f9dca67454f647c9ac710a500a0bbebb@sentry.indeed.com
+          <t xml:space="preserve">nr@context
+nr@id
+20@treepeople
+20@treepeople
 </t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.simplyhired.com/search%3Fq%3Dmicrosoft%26l%3Dredmond%252C%2Bwa</t>
+          <t>https://www.treepeople.org/tree-benefits</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Highest paying jobs at Microsoft</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mingraham@theladders.com.
-mingraham@theladders.com
-mlepore@theladders.com.
-mlepore@theladders.com
-udc9e@fashncurious
-mlepore@theladders.com.
-mlepore@theladders.com
-eprice@theladders.com
-jfabiano@theladders.com
-mlepore@theladders.com.
-mlepore@theladders.com
-u00a0@nytimes
-u00a0@genderfair
-u00a0@janssenglobal
-u00a0@janssenglobal
-mlepore@theladders.com.
-mlepore@theladders.com
-agarrido@theladders.com
-susannakahr@theladders.com
-</t>
-        </is>
-      </c>
+          <t>https://www.youtube.com/watch%3Fv%3DHPJKxAhLw5I</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>2144</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
-        <v>318</v>
+        <v>0</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.theladders.com/company/microsoft-jobs</t>
+          <t>https://www.youtube.com/watch%3Fv%3DHPJKxAhLw5I</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed google web-scrape to google search module
</commit_message>
<xml_diff>
--- a/ShawnTestData.xlsx
+++ b/ShawnTestData.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -386,287 +386,488 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Programming Jobs, Employment in Colorado Springs, CO | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed.com
+</t>
+        </is>
+      </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1604</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://t1.gstatic.com/images%3Fq%3Dtbn:ANd9GcQ2lQIXSBhSUrZ4g27utbm8yvu6bz-3v9S9TF-ZWHPH_-5NggdM</t>
+          <t>https://www.indeed.com/q-Programming-l-Colorado-Springs,-CO-jobs.html</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cats (musical) - Wikipedia</t>
+          <t>Computer Programming Jobs, Employment in Colorado | Indeed.com</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">tokens@tffin
+          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed.com
 </t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>1616</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="E3" t="n">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://en.wikipedia.org/wiki/Cats_(musical)</t>
+          <t>https://www.indeed.com/q-Computer-Programming-l-Colorado-jobs.html</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch%3Fv%3DgNTDoOmc1OQ</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+          <t>Computer Programmer Jobs, Employment in Colorado Springs, CO | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed.com
+</t>
+        </is>
+      </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1457</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>130</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch%3Fv%3DgNTDoOmc1OQ</t>
+          <t>https://www.indeed.com/q-Computer-Programmer-l-Colorado-Springs,-CO-jobs.html</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>403 Forbidden</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
+          <t>Programmer Jobs, Employment | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed.com
+</t>
+        </is>
+      </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1602</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.catsthemusical.com/</t>
+          <t>https://www.indeed.com/q-Programmer-jobs.html</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TryIMDbProFree</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mv5bnte4nwrhymqtoty4ys00owmwlwewywutzjvjndhhodc5yznmxkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bnte4nwrhymqtoty4ys00owmwlwewywutzjvjndhhodc5yznmxkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bnte4nwrhymqtoty4ys00owmwlwewywutzjvjndhhodc5yznmxkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bztnkzmu0zwqtzjqzmy00ytnmlwfmn2mtzgnkmmu1othmmgywxkeyxkfqcgdeqxvynzkwmjq5nzm@.
-mv5bmjq1njm3mtuxnv5bml5banbnxkftztgwmdc5mty5ote@.
-mv5bzdawytlhmdetntg0os00ndy2lwjjowitnwy3ytzkm2uxyzuzxkeyxkfqcgdeqxvynta4nzy1mzy@.
-mv5bnte4nwrhymqtoty4ys00owmwlwewywutzjvjndhhodc5yznmxkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bnzfmotazogutntg3nc00ngrmltg1mgitnwnhzte4yza3ntrll2ltywdll2ltywdlxkeyxkfqcgdeqxvymtq2oduxmjq@.
-mv5bmdljntq5oditzmqwmy00m2exltljotqtztvjnge2ntg0ngixxkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bmty1odi5nzq1nf5bml5banbnxkftztgwmzq5ndm5ntm@.
-mv5bmjmxodi2ndm5nl5bml5banbnxkftztgwnjgzotk1mti@.
-mv5bnji5otnkmzutzdyzyy00nwq5ltg4yzytzmzjzdi0mgqzngy2xkeyxkfqcgdeqxvynjg2njqwmdq@.
-mv5bmjiwmje1nzc4nv5bml5banbnxkftztgwndg4ota1nzm@.
-mv5bogizyjm3yzmtmjk5zs00ndy2ltllmjetnjywzjhmmdnhmdbkxkeyxkfqcgdeqxvyoduzmjqxmta@.
-mv5bogqyotq1ntqtmznkzs00ndbilwe5otgtyzg4mmu5mwi1ndy4xkeyxkfqcgdeqxvyntc5otmwotq@.
-mv5botywzta3nzutngzlys00zdlllwjjmzutogfhmzbhntnlmwezxkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bzwrlzduxyjetztg1mi00mdq2lwewotetotg3ymu3ndcwmja5xkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bm2jlm2m1nzmtztjlns00ymiylwjkowutzmzkn2nhmwfjzjc2xkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5byjmwyzi2zmytowi3my00mtfilwi2ndmtodqyyta0ywnjotrhxkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bn2u3zjdimzutymi5mi00otc2lwjlnzytnzi4mtmwotbjmgy4xkeyxkfqcgdeqxvyodq2nduxnzk@.
-mv5bnzg1mzm3owutnjgzzc00njmzlwe1nzatothimdgymjhhzdbhxkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bmji2nze5mzq4n15bml5banbnxkftztgwndewndm4njm@.
-mv5bmja0yjyyzgmtn2u0ni00ymy4lwjkztitytmymjy3ngyymtjkxkeyxkfqcgdeqxvyndg4njy5otq@.
-mv5bntg4yjqymdatzwfiyi00otmzlwjiytgtmzrinwmzmtazmdq0xkeyxkfqcgdeqxvynjg2njqwmdq@.
-mv5bndc1ztlmowutndy2ys00ogu5ltg2mtytytk2mmqzmge2nzuwxkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bndc4njyzowitymuzyy00mta3lthimtctntlizdlky2fjzjrlxkeyxkfqcgdeqxvyndg4njy5otq@.
-mv5bywm1zdq5yzctowi4yi00ymq3lthkmtctmgm5mtc0zwnhodhjxkeyxkfqcgdeqxvyndg4njy5otq@.
-mv5bnzg1mzm3owutnjgzzc00njmzlwe1nzatothimdgymjhhzdbhxkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bmji2nze5mzq4n15bml5banbnxkftztgwndewndm4njm@.
-mv5bmja0yjyyzgmtn2u0ni00ymy4lwjkztitytmymjy3ngyymtjkxkeyxkfqcgdeqxvyndg4njy5otq@.
-mv5bntg4yjqymdatzwfiyi00otmzlwjiytgtmzrinwmzmtazmdq0xkeyxkfqcgdeqxvynjg2njqwmdq@.
-mv5bndc1ztlmowutndy2ys00ogu5ltg2mtytytk2mmqzmge2nzuwxkeyxkfqcgdeqxvyodkzntgxmdg@.
-mv5bndc4njyzowitymuzyy00mta3lthimtctntlizdlky2fjzjrlxkeyxkfqcgdeqxvyndg4njy5otq@.
-mv5bywm1zdq5yzctowi4yi00ymq3lthkmtctmgm5mtc0zwnhodhjxkeyxkfqcgdeqxvyndg4njy5otq@.
-mv5bmjeymtizoti2ov5bml5banbnxkftztgwntyxmjc0nte@.
-mv5bmtcymda2mtgwmf5bml5banbnxkftztgwodgyndm2nde@.
-mv5bzjeyyjyymwutztm0zs00yji0lwi0ngutmjqyy2vmnta3yjnhxkeyxkfqcgdeqxvyotq2njy0nzc@.
-mv5bmgnkymuzowetzjk2my00ytvilwfknzutodgwmti5nmzizwvixkeyxkfqcgdeqxvyote0njgwmjy@.
-mv5bzjgzywzimtgtzguzoc00zwjmltkxotgtogm0zjbjnjhjyzq4xkeyxkfqcgdeqxvyotizntqyoda@.
-mv5bmtk0nzawmtuwm15bml5banbnxkftztgwntqzodmwode@.
-mv5bntjkyjriymmtodzhms00zjyylwixmwetmtmymgu3mgvkyjblxkeyxkfqcgdeqxvyote0njgwmjy@.
-mv5bmzuzndm2nzm2mv5bml5banbnxkftztgwntm3ntg4ote@.
-mv5bmmu3nziyodctyjvhoc00nzbmltlhnwitmzblodewztlmmjuzxkeyxkfqcgdeqxvyntizotk5odm@.
-mv5bzwixnzm5yzqty2fmms00yjc3lwi1zjutngvjmjmzztixztixxkeyxkfqcgdeqxvynju0otq0oty@.
-mv5bmjezoda3mdcxml5bml5banbnxkftztgwodgxndk3nze@.
-mv5bndyynzk1nzywof5bml5banbnxkftztgwmtq0nzc4mzi@.
-mv5bnzqynjlkmtitnzaxnc00yzm4ltk3njktzjm2nzdlmzi3mwywxkeyxkfqcgdeqxvynjkwnzewmzu@.
-mv5byju1yty1yzitnmqyys00mwrklwfiogityjm4zgjiytkxmdg2xkeyxkfqcgdeqxvyoduxotu0otg@.
-mv5bmtk1mjyzotu2nl5bml5banbnxkftztgwmzaxmtg5mte@.
-</t>
-        </is>
-      </c>
+          <t>Apache Tomcat - Error report</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.imdb.com/title/tt5697572/</t>
+          <t>https://www.glassdoor.com/job-listing/java-programmer-digital-prospectors-JV_IC1148136_KO0,15_KE16,35.htm?jl=3215493909</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">nr@context
-nr@id
-izadi@washpost.com
-readers@washpost.com
-legro@washpost.com
-izadi@washpost.com
-izadi@washpost.com
-izadi@washpost.com
-izadi@washpost.com
-izadi@washpost.com
-andrewst@washpost.com
-</t>
-        </is>
-      </c>
+          <t>$53k-$103k Software Programming Jobs in Colorado Springs, CO</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>1401</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.washingtonpost.com/arts-entertainment/2019/11/19/new-cats-trailer-is-here-its-time-discuss-these-cat-bodies/</t>
+          <t>https://www.ziprecruiter.com/Jobs/Software-Programming/-in-Colorado-Springs,CO</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
+          <t>$45k-$74k Computer Programmer Jobs in Colorado | ZipRecruiter</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>1444</v>
+      </c>
+      <c r="D8" t="n">
+        <v>110</v>
+      </c>
+      <c r="E8" t="n">
+        <v>47</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.ziprecruiter.com/Jobs/Computer-Programmer/--in-Colorado</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Revature hiring Entry Level Programmer - in Colorado Springs, CO, US | LinkedIn</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>833</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" t="n">
+        <v>21</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/view/entry-level-programmer-at-revature-1229869177</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Remote Programming Jobs</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t xml:space="preserve">nr@context
 nr@id
 nr@original
-logo@2x.png
+you@youremail.com
+you@youremail.com
+logov2@2x
+logov2@2x
+hello@tinyboards.co
+matt@tinyboards.co
 </t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>8</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>https://www.purina.com/cats/cat-breeds</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Complete Guide to Caring for Cats | Cat Breed Information, Cat Training, Cat Grooming</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>http://www.vetstreet.com/cats/</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>'Cats' trailer: Taylor Swift, Idris Elba inspire fresh feline jokes</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">logo@2x.png
-ros@970x250
-video@920x508
-ros@300x1050
-ros@300x1050
-btf@728x90
-</t>
-        </is>
-      </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>350</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.usatoday.com/story/entertainment/movies/2019/11/19/cats-new-trailer-brings-more-taylor-swift-idris-elba-jokes/4239562002/</t>
+          <t>https://weworkremotely.com/categories/remote-programming-jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>21 Best Websites To Get Programming Jobs In 2019</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">feedback@forbes.com
+corrections@forbes.com
+abdullahi@oxygenmat.net
+abdullahi@oxygenmat.net
+</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>353</v>
+      </c>
+      <c r="D11" t="n">
+        <v>15</v>
+      </c>
+      <c r="E11" t="n">
+        <v>54</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://www.forbes.com/sites/abdullahimuhammed/2019/10/08/21-best-websites-to-get-programming-jobs-in-2019/</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Top 20 programming jobs, Now Hiring | Dice.com</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">email@domain.com
+newdicesupport@dice.com
+newdicesupport@dice.com
+</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>752</v>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="n">
+        <v>164</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://www.dice.com/jobs/q-programming-jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12+ High Paying Technology Jobs for Software Engineers and Computer Programmers - By Javin Paul</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">vue@2.6.10
+support@hackernoon.com
+cookie@2
+</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>44</v>
+      </c>
+      <c r="D13" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" t="n">
+        <v>33</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://hackernoon.com/12-high-paying-technology-jobs-for-software-engineers-and-computer-programmers-8d72b6b1861c</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Flexible &amp; Telecommuting Programmer Jobs | FlexJobs</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>459</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E14" t="n">
+        <v>16</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://www.flexjobs.com/jobs/telecommuting-Programmer-jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Computer Programming Job Listings | Career Search | Monster.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>518</v>
+      </c>
+      <c r="D15" t="n">
+        <v>72</v>
+      </c>
+      <c r="E15" t="n">
+        <v>8</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://www.monster.com/jobs/q-computer-programming-jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>8 Programming Jobs With Top Salaries | Robert Half</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nr@seenerror
+nr@wrapped
+nr@context
+nr@context
+nr@id
+nr@original
+sample@test.com.
+sample@test.com
+</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>147</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" t="n">
+        <v>56</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.roberthalf.com/blog/compensation-and-benefits/big-bucks-4-programming-jobs-with-the-highest-salaries</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Computer Programmers: Jobs, Career, Salary and Education Information    </t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="n">
+        <v>85</v>
+      </c>
+      <c r="D17" t="n">
+        <v>122</v>
+      </c>
+      <c r="E17" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://collegegrad.com/careers/computer-programmers</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Getting That First Programming Job: Easier Than You Think | Adzerk</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>83</v>
+      </c>
+      <c r="D18" t="n">
+        <v>12</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://adzerk.com/blog/getting-first-programming-job/</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Computer Programmer Job Description: Salary, Skills, &amp; More</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="n">
+        <v>301</v>
+      </c>
+      <c r="D19" t="n">
+        <v>132</v>
+      </c>
+      <c r="E19" t="n">
+        <v>17</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://www.thebalancecareers.com/computer-programmer-job-description-salary-and-skills-2061823</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>icon-util-x</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>94</v>
+      </c>
+      <c r="D20" t="n">
+        <v>38</v>
+      </c>
+      <c r="E20" t="n">
+        <v>137</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://www.rasmussen.edu/degrees/technology/blog/programming-careers-for-coding-connoisseurs/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a dictionary manager to merge the dictionary between dictionaries in different threads
</commit_message>
<xml_diff>
--- a/ShawnTestData.xlsx
+++ b/ShawnTestData.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -385,6 +385,250 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>20 Best jobs in Colorado Springs, CO (Hiring Now!) | SimplyHired</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">f9dca67454f647c9ac710a500a0bbebb@sentry.indeed.com
+</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>629</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://www.snagajob.com/search/w-colorado+springs,+co</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>All Jobs in Colorado Springs, CO - Apply Now | CareerBuilder</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>430</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>18</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://www.snagajob.com/search/w-colorado+springs,+co</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>$60,000 Jobs, Employment in Colorado Springs, CO | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed.com
+</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1471</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>22</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://www.snagajob.com/search/w-colorado+springs,+co</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Jobs, Employment in Colorado Springs, CO | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed.com
+</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1553</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>18</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://www.snagajob.com/search/w-colorado+springs,+co</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Apache Tomcat - Error report</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://www.snagajob.com/search/w-colorado+springs,+co</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>$34k-$81k Jobs in Colorado Springs, CO | ZipRecruiter</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>1452</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>12</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://www.snagajob.com/search/w-colorado+springs,+co</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LinkedIn Job Search: Find US Jobs, Internships, Jobs Near Me</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>475</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.snagajob.com/search/w-colorado+springs,+co</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Find a Job | Careers in Colorado Springs, CO | Monster</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>440</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://www.snagajob.com/search/w-colorado+springs,+co</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>City Jobs and Careers | Colorado Springs</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nr@context
+nr@id
+nr@original
+hr@springsgov.com
+webmaster@springsgov.com
+</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>59</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://www.snagajob.com/search/w-colorado+springs,+co</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Jobs in Colorado Springs, Co Now Hiring | Snagajob</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>431</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://www.snagajob.com/search/w-colorado+springs,+co</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Started Work on fixing emails
</commit_message>
<xml_diff>
--- a/ShawnTestData.xlsx
+++ b/ShawnTestData.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,159 +388,159 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Python Jobs, Employment in Colorado Springs, CO | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/q-Python-l-Colorado-Springs,-CO-jobs.html</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1551</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>87</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Python Jobs, Employment in Colorado | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/q-Python-l-Colorado-jobs.html</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1760</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>54</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Python Jobs, Employment | Indeed.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/q-Python-jobs.html</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1771</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>27</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>Python Job Board | Python.org</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>https://www.python.org/jobs/</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C5" t="n">
         <v>431</v>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
         <v>5</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t xml:space="preserve">jobs@python.org
 </t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Python Jobs, Employment in Colorado | Indeed.com</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://www.indeed.com/q-Python-l-Colorado-jobs.html</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1565</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>55</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed.com
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Python Jobs, Employment | Indeed.com</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://www.indeed.com/q-Python-jobs.html</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1590</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>35</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed.com
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Python Jobs, Employment in Colorado Springs, CO | Indeed.com</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://www.indeed.com/q-Python-l-Colorado-Springs,-CO-jobs.html</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1566</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>94</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed.com
-</t>
-        </is>
-      </c>
-    </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Xeenius, LLC hiring Python Developer in Englewood, CO, US | LinkedIn</t>
+          <t>Remote Data Engineer - Python Job in Colorado Springs, CO at The Hartford Financial Services Group, Inc</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/python-developer-at-xeenius-llc-1087542216</t>
+          <t>https://www.ziprecruiter.com/c/The-Hartford-Financial-Services-Group,-Inc/Job/Remote-Data-Engineer-Python/-in-Colorado-Springs,CO?jid=DO16f3b829cc7e78f74979bbb52ab0b18c</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1524</v>
+        <v>656</v>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Remote Data Engineer - Python Job in Colorado Springs, CO at The Hartford Financial Services Group, Inc</t>
+          <t>Xeenius, LLC hiring Python Developer in Englewood, CO, US | LinkedIn</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.ziprecruiter.com/c/The-Hartford-Financial-Services-Group,-Inc/Job/Remote-Data-Engineer-Python/-in-Colorado-Springs,CO?jid=DO16f3b829cc7e78f74979bbb52ab0b18c</t>
+          <t>https://www.linkedin.com/jobs/view/python-developer-at-xeenius-llc-1087542216</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>656</v>
+        <v>1524</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>108,000+ Python jobs in United States (2,408 new)</t>
+          <t>108,000+ Python jobs in United States (2,431 new)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -549,86 +549,428 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>$88k-$124k Python Developer Jobs in Colorado | ZipRecruiter</t>
+          <t>Just a moment...</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.ziprecruiter.com/Jobs/Python-Developer/--in-Colorado</t>
+          <t>https://www.pythonjobs.com/</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1445</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20 Best python jobs (Hiring Now!) | SimplyHired</t>
+          <t>Python Jobs in Colorado | Built In Colorado</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.simplyhired.com/search?q=python</t>
+          <t>https://www.builtincolorado.com/jobs?f[0]=job-category_developer-engineer-python</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>718</v>
+        <v>824</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>17</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">f9dca67454f647c9ac710a500a0bbebb@sentry.indeed.com
-</t>
-        </is>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Python Jobs in Colorado | Built In Colorado</t>
+          <t>20 Best python jobs (Hiring Now!) | SimplyHired</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.builtincolorado.com/jobs?f[0]=job-category_developer-engineer-python</t>
+          <t>https://www.simplyhired.com/search?q=python</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>824</v>
+        <v>643</v>
       </c>
       <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>12</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">f9dca67454f647c9ac710a500a0bbebb@sentry.indeed
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>$88k-$124k Python Developer Jobs in Colorado | ZipRecruiter</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.ziprecruiter.com/Jobs/Python-Developer/--in-Colorado</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1445</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>21</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Apache Tomcat - Error report</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://www.glassdoor.com/Job/us-python-jobs-SRCH_IL.0,2_IN1_KO3,9.htm</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Top 20 Python jobs, Now Hiring | Dice.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://www.dice.com/jobs/q-Python-jobs</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>742</v>
+      </c>
+      <c r="D14" t="n">
         <v>3</v>
       </c>
-      <c r="E11" t="n">
-        <v>121</v>
-      </c>
-      <c r="F11" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>118</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">email@domain.com
+newdicesupport@dice.com
+newdicesupport@dice.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Remote Python Jobs
+ | RemotePython.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.remotepython.com/jobs/</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>237</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">info@remotepython.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Python Jobs  - Stack Overflow</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://stackoverflow.com/jobs/developer-jobs-using-python</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1095</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6</v>
+      </c>
+      <c r="E16" t="n">
+        <v>33</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Access to this page has been denied.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.upwork.com/freelance-jobs/python/</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Python Jobs in NYC | Built In NYC</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://www.builtinnyc.com/jobs?f[0]=job-category_developer-engineer-python</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>865</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" t="n">
+        <v>103</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Flexible &amp; Telecommuting Python Jobs | FlexJobs</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://www.flexjobs.com/jobs/telecommuting-python-jobs</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>432</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+      <c r="F19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Attention Required! | Cloudflare</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://angel.co/python/jobs</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Remote Python Jobs in December 2019</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://remoteok.io/remote-python-jobs</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>10727</v>
+      </c>
+      <c r="D21" t="n">
+        <v>64</v>
+      </c>
+      <c r="E21" t="n">
+        <v>825</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello@geektastic.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Python Jobs, Please: The 8 Best Job Titles for Python Users - Skillcrush</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://skillcrush.com/2019/09/03/python-job-titles/</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>118</v>
+      </c>
+      <c r="D22" t="n">
+        <v>5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>54</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">logo@2x.png
+hello@skillcrush.com
+hello@skillcrush.com
+logo@2x.png
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Python Jobs - December 2019 | Indeed.co.uk</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://www.indeed.co.uk/Python-jobs</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1443</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>13</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0252655a41544fd28ae41f8b8ff36917@sentry.indeed
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+              Python Jobs for December 2019 | Freelancer
+          </t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://www.freelancer.com/jobs/python/</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1896</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" t="n">
+        <v>8</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Python Jobs - Apply Now | CareerBuilder</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://www.careerbuilder.com/jobs-python</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>431</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>20</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Changed variable iteration to row_num in main.py
</commit_message>
<xml_diff>
--- a/ShawnTestData.xlsx
+++ b/ShawnTestData.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,231 +388,225 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Python Job Board | Python.org</t>
+          <t>Forestry, Trees &amp; Timber Careers | AllAboutCareers</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.python.org/jobs/</t>
+          <t>https://www.allaboutcareers.com/careers/career-path/forestry-trees-timber</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>452</v>
+        <v>538</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Python Jobs, Employment in Colorado | Indeed.com</t>
+          <t>Visa</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/q-Python-l-Colorado-jobs.html</t>
+          <t>https://www.tentsile.com/blogs/news/5-awesome-careers-for-people-who-love-trees?sa=X&amp;ved=2ahUKEwjPhu3huZzmAhUNuZ4KHauQAZ4Q9QF6BAgLEAI</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1756</v>
+        <v>56</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>56</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">jgpmc59@gmail.com
+zulujrmoses@gmail.com
+info@tentsile.com
+support@tentsile.com
+support@tentsile.com
+repairs@tentsile.com
+repairs@tentsile.com
+info@tentsile.com
+</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Python Jobs, Employment in Colorado Springs, CO | Indeed.com</t>
+          <t>Tree Jobs, Employment | Indeed.com</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/q-Python-l-Colorado-Springs,-CO-jobs.html</t>
+          <t>https://www.indeed.com/q-Tree-jobs.html</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1473</v>
+        <v>1780</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Python Jobs in Colorado | Built In Colorado</t>
+          <t>Tree Service Jobs, Employment in Colorado | Indeed.com</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.builtincolorado.com/jobs?f[0]=job-category_developer-engineer-python</t>
+          <t>https://www.indeed.com/q-Tree-Service-l-Colorado-jobs.html</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>802</v>
+        <v>1777</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20 Best python jobs (Hiring Now!) | SimplyHired</t>
+          <t>50 Careers in Trees - Tree Foundation of Kern: About the Tree Foundation of Kern</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.simplyhired.com/search?q=python</t>
+          <t>http://www.urbanforest.org/index.cfm/fuseaction/Pages.Page/id/430</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>631</v>
+        <v>8</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Just a moment...</t>
+          <t>Job Opportunities - Friends of Trees</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.pythonjobs.com/</t>
+          <t>https://friendsoftrees.org/about/job-opportunities/</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Top 20 Python jobs, Now Hiring | Dice.com</t>
+          <t>20 Best tree felling jobs (Hiring Now!) | SimplyHired</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.dice.com/jobs/q-Python-jobs</t>
+          <t>https://www.simplyhired.com/search?q=tree+felling</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>767</v>
+        <v>633</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>117</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">email@domain.com
-newdicesupport@dice.com
-newdicesupport@dice.com
-</t>
-        </is>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>114,000+ Python jobs in United States (4,600 new)</t>
+          <t>Grist</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/python-jobs</t>
+          <t>https://grist.org/article/2010-02-01-the-jobs-are-in-the-trees/</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>702</v>
+        <v>74</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>$89k-$124k Python Developer Jobs in Colorado | ZipRecruiter</t>
+          <t>Green Jobs - Knowledge of Tree Care Career and Education.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.ziprecruiter.com/Jobs/Python-Developer/--in-Colorado</t>
+          <t>https://californiareleaf.org/resources/green-jobs/</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1447</v>
+        <v>64</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>27</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Remote Python Jobs in December 2019</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>https://remoteok.io/remote-python-jobs</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>10702</v>
-      </c>
-      <c r="D11" t="n">
-        <v>64</v>
-      </c>
-      <c r="E11" t="n">
-        <v>825</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hello@geektastic.com
+        <v>1</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">lforlin@peralta.edu
+lforlin@peralta.edu
+cbrey@aplustree.com
+cbrey@aplustree.com
+ckirkman@arborwell.com
+ckirkman@arborwell.com
+andrew.misch@davey.com
+andrew.misch@davey.com
+jbartolo@wcainc.com
+jbartolo@wcainc.com
+cdiaz@wcainc.com
+cdiaz@wcainc.com
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
Changed output to be more streamlined.
</commit_message>
<xml_diff>
--- a/ShawnTestData.xlsx
+++ b/ShawnTestData.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,228 +388,227 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Forestry, Trees &amp; Timber Careers | AllAboutCareers</t>
+          <t>Earn an Acoustic Engineering Degree | Acoustical Schools</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.allaboutcareers.com/careers/career-path/forestry-trees-timber</t>
+          <t>https://educatingengineers.com/degrees/acoustic-engineering</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>538</v>
+        <v>68</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Compare Industrial Engineering Courses and Degree Programs</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.tentsile.com/blogs/news/5-awesome-careers-for-people-who-love-trees?sa=X&amp;ved=2ahUKEwjPhu3huZzmAhUNuZ4KHauQAZ4Q9QF6BAgLEAI</t>
+          <t>https://educatingengineers.com/degrees/industrial-engineering</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">jgpmc59@gmail.com
-zulujrmoses@gmail.com
-info@tentsile.com
-support@tentsile.com
-support@tentsile.com
-repairs@tentsile.com
-repairs@tentsile.com
-info@tentsile.com
-</t>
-        </is>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tree Jobs, Employment | Indeed.com</t>
+          <t>Nuclear Engineering Schools and Degrees | EducatingEngineers.com</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/q-Tree-jobs.html</t>
+          <t>https://educatingengineers.com/degrees/nuclear-engineering</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1780</v>
+        <v>52</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tree Service Jobs, Employment in Colorado | Indeed.com</t>
+          <t>Civil Engineer Jobs and Careers | EducatingEngineers.com</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/q-Tree-Service-l-Colorado-jobs.html</t>
+          <t>https://educatingengineers.com/careers/civil-engineer</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1777</v>
+        <v>134</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="E5" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>50 Careers in Trees - Tree Foundation of Kern: About the Tree Foundation of Kern</t>
+          <t>8 Best Engineering Jobs | Best Jobs Rankings | US News Careers</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://www.urbanforest.org/index.cfm/fuseaction/Pages.Page/id/430</t>
+          <t>https://money.usnews.com/careers/best-jobs/rankings/best-engineering-jobs</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>661</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Job Opportunities - Friends of Trees</t>
+          <t>List of Engineering Career Options with Job Descriptions | EducatingEngineers.com</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://friendsoftrees.org/about/job-opportunities/</t>
+          <t>https://educatingengineers.com/career-specialties</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20 Best tree felling jobs (Hiring Now!) | SimplyHired</t>
+          <t>Engineering Careers: Options, Job Titles, and Descriptions</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.simplyhired.com/search?q=tree+felling</t>
+          <t>https://www.thebalancecareers.com/engineering-job-titles-2061493</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>633</v>
+        <v>339</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E8" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Grist</t>
+          <t xml:space="preserve">Top-paying jobs are in engineering </t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://grist.org/article/2010-02-01-the-jobs-are-in-the-trees/</t>
+          <t>https://money.cnn.com/2013/04/25/news/economy/engineering-best-paid-jobs/index.html?sa=X&amp;ved=2ahUKEwiS28uDwZzmAhUJPa0KHRRTAPQQ9QF6BAgLEAI</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Green Jobs - Knowledge of Tree Care Career and Education.</t>
+          <t>The Best Engineering Jobs for Engineers | ENGINEERING.com</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://californiareleaf.org/resources/green-jobs/</t>
+          <t>https://www.engineering.com/jobs/</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>64</v>
+        <v>362</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">lforlin@peralta.edu
-lforlin@peralta.edu
-cbrey@aplustree.com
-cbrey@aplustree.com
-ckirkman@arborwell.com
-ckirkman@arborwell.com
-andrew.misch@davey.com
-andrew.misch@davey.com
-jbartolo@wcainc.com
-jbartolo@wcainc.com
-cdiaz@wcainc.com
-cdiaz@wcainc.com
+          <t xml:space="preserve">support@engineering.com
 </t>
         </is>
       </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>The 6 Highest Paid Engineering Jobs</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://typesofengineeringdegrees.org/highest-paid-engineering-jobs/</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>95</v>
+      </c>
+      <c r="D11" t="n">
+        <v>37</v>
+      </c>
+      <c r="E11" t="n">
+        <v>13</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>